<commit_message>
update:trans and めめ村 skins
</commit_message>
<xml_diff>
--- a/VisorTransData.xlsx
+++ b/VisorTransData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7478160C-9AC8-495E-8214-1A8361F77F59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E504B3-C2D1-493B-A2A9-09D9DE51154D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hat" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>English</t>
   </si>
@@ -125,13 +125,21 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>ヒナメット1</t>
-  </si>
-  <si>
     <t>ルカメット</t>
   </si>
   <si>
     <t>LukaHead</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ヒナメット</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Gusao</t>
+  </si>
+  <si>
+    <t>ぐさお(本体)</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -472,7 +480,7 @@
   <dimension ref="A1:Q34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -556,30 +564,38 @@
         <v>20</v>
       </c>
       <c r="M7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="M9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
         <v>23</v>
       </c>
-      <c r="M10" t="s">
+      <c r="M11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A13" t="s">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
         <v>21</v>
       </c>
-      <c r="M13" t="s">
+      <c r="M14" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat:new visor. thunk you, 猫野和錆, Admin
</commit_message>
<xml_diff>
--- a/VisorTransData.xlsx
+++ b/VisorTransData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C9092A7-ADDF-4B04-BE14-57237D4325D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A547661-40BB-4284-9FCB-B559FF391E5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hat" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="73">
   <si>
     <t>English</t>
   </si>
@@ -290,12 +290,39 @@
     <t>jitome</t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>surprised</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>驚愕</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Admin</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Admin作</t>
+    <rPh sb="5" eb="6">
+      <t>サク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bluefire</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>邪眼が疼くぜ</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -309,12 +336,6 @@
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFCE9178"/>
-      <name val="Consolas"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -337,12 +358,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -625,16 +643,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q35"/>
+  <dimension ref="A1:Q40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="30.625" customWidth="1"/>
-    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="2" max="2" width="13.125" customWidth="1"/>
     <col min="13" max="13" width="38.875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -705,206 +723,227 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A6" s="2"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="M7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
-        <v>26</v>
-      </c>
-      <c r="M8" t="s">
-        <v>25</v>
+      <c r="A6" t="s">
+        <v>71</v>
+      </c>
+      <c r="M6" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="M9" t="s">
-        <v>29</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="M10" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
         <v>23</v>
       </c>
-      <c r="M11" t="s">
+      <c r="M13" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A14" t="s">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
         <v>21</v>
       </c>
-      <c r="M14" t="s">
+      <c r="M16" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A16" s="1">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A18" s="1">
         <v>1001001</v>
       </c>
-      <c r="M16" t="s">
+      <c r="M18" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A17" t="s">
-        <v>32</v>
-      </c>
-      <c r="M17" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A18" t="s">
-        <v>34</v>
-      </c>
-      <c r="M18" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="M19" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="M20" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="M21" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="M22" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="M23" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
+        <v>40</v>
+      </c>
+      <c r="M24" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A25" t="s">
+        <v>42</v>
+      </c>
+      <c r="M25" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A26" t="s">
         <v>44</v>
       </c>
-      <c r="M24" t="s">
+      <c r="M26" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A25" s="1" t="s">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A27" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="M25" t="s">
+      <c r="M27" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A26" s="1" t="s">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A28" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="M26" t="s">
+      <c r="M28" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A27" t="s">
-        <v>48</v>
-      </c>
-      <c r="M27" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A28" t="s">
-        <v>51</v>
-      </c>
-      <c r="M28" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="M29" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="M30" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A31" s="1" t="s">
-        <v>57</v>
+      <c r="A31" t="s">
+        <v>53</v>
       </c>
       <c r="M31" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="M32" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A33" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="M33" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A34" s="1" t="s">
-        <v>63</v>
+      <c r="A34" t="s">
+        <v>59</v>
       </c>
       <c r="M34" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A35" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M35" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A36" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M36" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A37" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="M35" t="s">
+      <c r="M37" t="s">
         <v>65</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A39" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="M39" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A40" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="M40" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat:new visor from oyakimon
</commit_message>
<xml_diff>
--- a/VisorTransData.xlsx
+++ b/VisorTransData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D7BAF11-B632-4243-80BC-7CBEC6B655BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F7B92F5-20A5-4597-8CDA-07AC508DCD55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="97">
   <si>
     <t>English</t>
   </si>
@@ -380,6 +380,34 @@
   <si>
     <t>YJBigEye</t>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>kuwa</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>くわっ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ワァ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>minidekawaii</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>oyaki</t>
+  </si>
+  <si>
+    <t>おやき</t>
+  </si>
+  <si>
+    <t>onsen</t>
+  </si>
+  <si>
+    <t>10秒で書いた</t>
   </si>
 </sst>
 </file>
@@ -707,16 +735,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q48"/>
+  <dimension ref="A1:Q59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="30.625" customWidth="1"/>
-    <col min="2" max="2" width="13.125" customWidth="1"/>
+    <col min="2" max="2" width="7" customWidth="1"/>
     <col min="13" max="13" width="38.875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -794,284 +822,316 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A9" t="s">
-        <v>20</v>
-      </c>
-      <c r="M9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A10" t="s">
-        <v>26</v>
-      </c>
-      <c r="M10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A11" t="s">
-        <v>28</v>
-      </c>
-      <c r="M11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A13" t="s">
-        <v>23</v>
-      </c>
-      <c r="M13" t="s">
-        <v>24</v>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>92</v>
+      </c>
+      <c r="M7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>89</v>
+      </c>
+      <c r="M8" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M16" t="s">
-        <v>22</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="M17" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A18" s="1">
-        <v>1001001</v>
+      <c r="A18" t="s">
+        <v>28</v>
       </c>
       <c r="M18" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A19" t="s">
-        <v>32</v>
-      </c>
-      <c r="M19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="M20" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A21" t="s">
-        <v>36</v>
-      </c>
-      <c r="M21" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A22" t="s">
-        <v>37</v>
-      </c>
-      <c r="M22" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="M23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A24" t="s">
-        <v>40</v>
-      </c>
-      <c r="M24" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A25" t="s">
-        <v>42</v>
+      <c r="A25" s="1">
+        <v>1001001</v>
       </c>
       <c r="M25" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="M26" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A27" s="1" t="s">
-        <v>66</v>
+      <c r="A27" t="s">
+        <v>34</v>
       </c>
       <c r="M27" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A28" s="1" t="s">
-        <v>46</v>
+      <c r="A28" t="s">
+        <v>36</v>
       </c>
       <c r="M28" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="M29" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="M30" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="M31" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="M32" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A33" s="1" t="s">
-        <v>57</v>
+      <c r="A33" t="s">
+        <v>44</v>
       </c>
       <c r="M33" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A34" t="s">
-        <v>59</v>
+      <c r="A34" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="M34" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A35" s="1" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="M35" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A36" s="1" t="s">
-        <v>63</v>
+      <c r="A36" t="s">
+        <v>48</v>
       </c>
       <c r="M36" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A37" s="1" t="s">
-        <v>64</v>
+      <c r="A37" t="s">
+        <v>51</v>
       </c>
       <c r="M37" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A38" s="1" t="s">
-        <v>73</v>
+      <c r="A38" t="s">
+        <v>53</v>
       </c>
       <c r="M38" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A39" s="1" t="s">
-        <v>75</v>
+      <c r="A39" t="s">
+        <v>55</v>
       </c>
       <c r="M39" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A40" s="1" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="M40" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A41" s="1" t="s">
-        <v>84</v>
+      <c r="A41" t="s">
+        <v>59</v>
       </c>
       <c r="M41" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A42" s="1" t="s">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="M42" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A43" s="1" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="M43" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A44" s="1" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="M44" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A45" s="1" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="M45" t="s">
-        <v>83</v>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A46" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="M46" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A47" s="1" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="M47" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A48" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="M48" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A49" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="M49" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A50" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="M50" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A51" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="M51" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A52" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="M52" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A54" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="M54" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A55" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="M48" t="s">
+      <c r="M55" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A58" t="s">
+        <v>93</v>
+      </c>
+      <c r="M58" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A59" t="s">
+        <v>95</v>
+      </c>
+      <c r="M59" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>